<commit_message>
Update issue 226: Pipeline:   Remove unused shaderregs.h dependency.   Some SSE optimization for         vs_output_ops::unproject_n,         vs_output_ops::selfintegral1_n and vs_output_ops::copy_n.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance.xlsx
+++ b/doc/contents/materials/PipelinePerformance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="20130105-PartOfSponza-Debug" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>v1227</t>
+  </si>
+  <si>
+    <t>v1231</t>
+  </si>
+  <si>
+    <t>v1331</t>
   </si>
 </sst>
 </file>
@@ -106,7 +112,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="6">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -131,33 +137,6 @@
       <fill>
         <patternFill>
           <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -555,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -577,6 +556,9 @@
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="C1" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="1">
@@ -585,6 +567,9 @@
       <c r="B2" s="1">
         <v>5080</v>
       </c>
+      <c r="C2" s="1">
+        <v>5022</v>
+      </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="1">
@@ -593,6 +578,9 @@
       <c r="B3" s="1">
         <v>5039</v>
       </c>
+      <c r="C3" s="1">
+        <v>4972</v>
+      </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="1">
@@ -601,6 +589,9 @@
       <c r="B4" s="1">
         <v>5049</v>
       </c>
+      <c r="C4" s="1">
+        <v>4957</v>
+      </c>
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="1">
@@ -609,6 +600,9 @@
       <c r="B5" s="1">
         <v>5068</v>
       </c>
+      <c r="C5" s="1">
+        <v>4935</v>
+      </c>
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="1">
@@ -617,6 +611,9 @@
       <c r="B6" s="1">
         <v>5083</v>
       </c>
+      <c r="C6" s="1">
+        <v>4943</v>
+      </c>
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="1">
@@ -625,6 +622,9 @@
       <c r="B7" s="1">
         <v>5081</v>
       </c>
+      <c r="C7" s="1">
+        <v>4969</v>
+      </c>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="1">
@@ -633,6 +633,9 @@
       <c r="B8" s="1">
         <v>5066</v>
       </c>
+      <c r="C8" s="1">
+        <v>4946</v>
+      </c>
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="1">
@@ -641,6 +644,9 @@
       <c r="B9" s="1">
         <v>5006</v>
       </c>
+      <c r="C9" s="1">
+        <v>4980</v>
+      </c>
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="1">
@@ -649,6 +655,9 @@
       <c r="B10" s="1">
         <v>5055</v>
       </c>
+      <c r="C10" s="1">
+        <v>4965</v>
+      </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="1">
@@ -657,6 +666,9 @@
       <c r="B11" s="1">
         <v>5050</v>
       </c>
+      <c r="C11" s="1">
+        <v>4931</v>
+      </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="1" t="s">
@@ -666,6 +678,26 @@
         <f>AVERAGE(B2:B11)</f>
         <v>5057.7</v>
       </c>
+      <c r="C12" s="3">
+        <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
+        <v>4962</v>
+      </c>
+      <c r="D12" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E12" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F12" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G12" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
@@ -675,6 +707,26 @@
         <f>_xlfn.VAR.S(B2:B11)</f>
         <v>557.78888888888889</v>
       </c>
+      <c r="C13" s="3">
+        <f t="shared" ref="C13:G13" si="1">_xlfn.VAR.S(C2:C11)</f>
+        <v>712.66666666666663</v>
+      </c>
+      <c r="D13" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E13" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F13" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G13" s="3" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" s="1" t="s">
@@ -683,9 +735,9 @@
       <c r="B14" s="1">
         <v>0</v>
       </c>
-      <c r="C14" s="1" t="e">
+      <c r="C14" s="1">
         <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>0.99999988359585479</v>
       </c>
       <c r="D14" s="1" t="e">
         <f>1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
@@ -711,9 +763,9 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="e">
+      <c r="C15" s="1">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>1.0192865779927449</v>
       </c>
       <c r="D15" s="1" t="e">
         <f>C12/D12</f>
@@ -740,9 +792,9 @@
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="e">
+      <c r="C16" s="1">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>1.0192865779927449</v>
       </c>
       <c r="D16" s="1" t="e">
         <f>B12/D12</f>
@@ -894,13 +946,13 @@
   <dataConsolidate/>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -914,10 +966,13 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
@@ -926,7 +981,9 @@
       <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -939,7 +996,9 @@
       <c r="B2" s="1">
         <v>87</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>92</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -952,7 +1011,9 @@
       <c r="B3" s="1">
         <v>86</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>93</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -965,7 +1026,9 @@
       <c r="B4" s="1">
         <v>88</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>92</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -978,7 +1041,9 @@
       <c r="B5" s="1">
         <v>87</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>92</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -991,7 +1056,9 @@
       <c r="B6" s="1">
         <v>95</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>92</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1004,7 +1071,9 @@
       <c r="B7" s="1">
         <v>87</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>93</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1017,7 +1086,9 @@
       <c r="B8" s="1">
         <v>86</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>93</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1030,7 +1101,9 @@
       <c r="B9" s="1">
         <v>88</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>93</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1043,7 +1116,9 @@
       <c r="B10" s="1">
         <v>87</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>95</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1056,7 +1131,9 @@
       <c r="B11" s="1">
         <v>86</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>93</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1070,9 +1147,9 @@
         <f>AVERAGE(B2:B11)</f>
         <v>87.7</v>
       </c>
-      <c r="C12" s="3" t="e">
+      <c r="C12" s="3">
         <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>92.8</v>
       </c>
       <c r="D12" s="3" t="e">
         <f t="shared" si="0"/>
@@ -1099,9 +1176,9 @@
         <f>_xlfn.VAR.S(B2:B11)</f>
         <v>7.1222222222222218</v>
       </c>
-      <c r="C13" s="3" t="e">
+      <c r="C13" s="3">
         <f t="shared" ref="C13:G13" si="1">_xlfn.VAR.S(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>0.84444444444444433</v>
       </c>
       <c r="D13" s="3" t="e">
         <f t="shared" si="1"/>
@@ -1127,9 +1204,9 @@
       <c r="B14" s="1">
         <v>0</v>
       </c>
-      <c r="C14" s="1" t="e">
+      <c r="C14" s="1">
         <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>0.99986942448991734</v>
       </c>
       <c r="D14" s="1" t="e">
         <f>1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
@@ -1155,9 +1232,9 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="e">
+      <c r="C15" s="1">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>0.94504310344827591</v>
       </c>
       <c r="D15" s="1" t="e">
         <f>C12/D12</f>
@@ -1183,9 +1260,9 @@
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="e">
+      <c r="C16" s="1">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>0.94504310344827591</v>
       </c>
       <c r="D16" s="1" t="e">
         <f>B12/D12</f>
@@ -1206,13 +1283,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B15:G16">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1224,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update issue 226: SALVIA:   Update performance document.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance.xlsx
+++ b/doc/contents/materials/PipelinePerformance.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="20130105-PartOfSponza-Debug" sheetId="1" r:id="rId1"/>
-    <sheet name="20130105-PartOfSponza-Release" sheetId="4" r:id="rId2"/>
+    <sheet name="PartOfSponza-Debug" sheetId="1" r:id="rId1"/>
+    <sheet name="PartOfSponza-Release" sheetId="4" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -48,7 +48,7 @@
     <t>v1231</t>
   </si>
   <si>
-    <t>v1331</t>
+    <t>v1232</t>
   </si>
 </sst>
 </file>
@@ -534,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -557,7 +557,7 @@
         <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -984,7 +984,9 @@
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -999,7 +1001,9 @@
       <c r="C2" s="1">
         <v>92</v>
       </c>
-      <c r="D2" s="1"/>
+      <c r="D2" s="1">
+        <v>75</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1014,7 +1018,9 @@
       <c r="C3" s="1">
         <v>93</v>
       </c>
-      <c r="D3" s="1"/>
+      <c r="D3" s="1">
+        <v>76</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1029,7 +1035,9 @@
       <c r="C4" s="1">
         <v>92</v>
       </c>
-      <c r="D4" s="1"/>
+      <c r="D4" s="1">
+        <v>76</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1044,7 +1052,9 @@
       <c r="C5" s="1">
         <v>92</v>
       </c>
-      <c r="D5" s="1"/>
+      <c r="D5" s="1">
+        <v>76</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1059,7 +1069,9 @@
       <c r="C6" s="1">
         <v>92</v>
       </c>
-      <c r="D6" s="1"/>
+      <c r="D6" s="1">
+        <v>76</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1074,7 +1086,9 @@
       <c r="C7" s="1">
         <v>93</v>
       </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1">
+        <v>75</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1089,7 +1103,9 @@
       <c r="C8" s="1">
         <v>93</v>
       </c>
-      <c r="D8" s="1"/>
+      <c r="D8" s="1">
+        <v>76</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1104,7 +1120,9 @@
       <c r="C9" s="1">
         <v>93</v>
       </c>
-      <c r="D9" s="1"/>
+      <c r="D9" s="1">
+        <v>75</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1119,7 +1137,9 @@
       <c r="C10" s="1">
         <v>95</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1">
+        <v>75</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1134,7 +1154,9 @@
       <c r="C11" s="1">
         <v>93</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1">
+        <v>75</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1151,9 +1173,9 @@
         <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
         <v>92.8</v>
       </c>
-      <c r="D12" s="3" t="e">
+      <c r="D12" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>75.5</v>
       </c>
       <c r="E12" s="3" t="e">
         <f t="shared" si="0"/>
@@ -1180,9 +1202,9 @@
         <f t="shared" ref="C13:G13" si="1">_xlfn.VAR.S(C2:C11)</f>
         <v>0.84444444444444433</v>
       </c>
-      <c r="D13" s="3" t="e">
+      <c r="D13" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.27777777777777779</v>
       </c>
       <c r="E13" s="3" t="e">
         <f t="shared" si="1"/>
@@ -1208,9 +1230,9 @@
         <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
         <v>0.99986942448991734</v>
       </c>
-      <c r="D14" s="1" t="e">
+      <c r="D14" s="1">
         <f>1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="E14" s="1" t="e">
         <f>1-_xlfn.T.TEST(D2:D11,E2:E11,2,3)</f>
@@ -1236,9 +1258,9 @@
         <f>B12/C12</f>
         <v>0.94504310344827591</v>
       </c>
-      <c r="D15" s="1" t="e">
+      <c r="D15" s="1">
         <f>C12/D12</f>
-        <v>#DIV/0!</v>
+        <v>1.2291390728476821</v>
       </c>
       <c r="E15" s="1" t="e">
         <f>D12/E12</f>
@@ -1264,9 +1286,9 @@
         <f>B12/C12</f>
         <v>0.94504310344827591</v>
       </c>
-      <c r="D16" s="1" t="e">
+      <c r="D16" s="1">
         <f>B12/D12</f>
-        <v>#DIV/0!</v>
+        <v>1.16158940397351</v>
       </c>
       <c r="E16" s="1" t="e">
         <f>B12/E12</f>

</xml_diff>

<commit_message>
Update issue 226 SALVIA:   Fixed bug of host_impl::vx_set_constant when cpp shader is enabled.   Fixed bugs of Benchmark* when cpp shader is enabled.   Update performance document.
</commit_message>
<xml_diff>
--- a/doc/contents/materials/PipelinePerformance.xlsx
+++ b/doc/contents/materials/PipelinePerformance.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="PartOfSponza" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>Test</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>v1242</t>
+  </si>
+  <si>
+    <t>v1243</t>
   </si>
 </sst>
 </file>
@@ -115,61 +118,7 @@
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -618,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -643,7 +592,9 @@
       <c r="E1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2"/>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
@@ -662,7 +613,9 @@
       <c r="E2" s="1">
         <v>80</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="1">
+        <v>102</v>
+      </c>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
@@ -681,7 +634,9 @@
       <c r="E3" s="1">
         <v>82</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="1">
+        <v>102</v>
+      </c>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7">
@@ -700,7 +655,9 @@
       <c r="E4" s="1">
         <v>80</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="1">
+        <v>103</v>
+      </c>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
@@ -719,7 +676,9 @@
       <c r="E5" s="1">
         <v>80</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1">
+        <v>101</v>
+      </c>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7">
@@ -738,7 +697,9 @@
       <c r="E6" s="1">
         <v>82</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1">
+        <v>103</v>
+      </c>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7">
@@ -757,7 +718,9 @@
       <c r="E7" s="1">
         <v>80</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1">
+        <v>101</v>
+      </c>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7">
@@ -776,7 +739,9 @@
       <c r="E8" s="1">
         <v>80</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="1">
+        <v>102</v>
+      </c>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7">
@@ -795,7 +760,9 @@
       <c r="E9" s="1">
         <v>80</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="1">
+        <v>102</v>
+      </c>
       <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7">
@@ -814,7 +781,9 @@
       <c r="E10" s="1">
         <v>80</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="1">
+        <v>102</v>
+      </c>
       <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7">
@@ -833,7 +802,9 @@
       <c r="E11" s="1">
         <v>80</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1">
+        <v>101</v>
+      </c>
       <c r="G11" s="1"/>
     </row>
     <row r="12" spans="1:7">
@@ -856,9 +827,9 @@
         <f t="shared" si="0"/>
         <v>80.400000000000006</v>
       </c>
-      <c r="F12" s="3" t="e">
+      <c r="F12" s="3">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
+        <v>101.9</v>
       </c>
       <c r="G12" s="3" t="e">
         <f t="shared" si="0"/>
@@ -885,9 +856,9 @@
         <f t="shared" si="1"/>
         <v>0.71111111111111114</v>
       </c>
-      <c r="F13" s="3" t="e">
+      <c r="F13" s="3">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>0.54444444444444451</v>
       </c>
       <c r="G13" s="3" t="e">
         <f t="shared" si="1"/>
@@ -913,9 +884,9 @@
         <f>1-_xlfn.T.TEST(D2:D11,E2:E11,2,3)</f>
         <v>0.99999999989732213</v>
       </c>
-      <c r="F14" s="1" t="e">
+      <c r="F14" s="1">
         <f>1-_xlfn.T.TEST(D2:D11,F2:F11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="G14" s="1" t="e">
         <f>1-_xlfn.T.TEST(F2:F11,G2:G11,2,3)</f>
@@ -941,9 +912,9 @@
         <f>D12/E12</f>
         <v>0.93905472636815912</v>
       </c>
-      <c r="F15" s="1" t="e">
+      <c r="F15" s="1">
         <f>D12/F12</f>
-        <v>#DIV/0!</v>
+        <v>0.7409224730127576</v>
       </c>
       <c r="G15" s="1" t="e">
         <f>F12/G12</f>
@@ -969,9 +940,9 @@
         <f>B12/E12</f>
         <v>1.0907960199004976</v>
       </c>
-      <c r="F16" s="1" t="e">
+      <c r="F16" s="1">
         <f>B12/F12</f>
-        <v>#DIV/0!</v>
+        <v>0.86064769381746808</v>
       </c>
       <c r="G16" s="1" t="e">
         <f>B12/G12</f>
@@ -998,8 +969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1011,7 +982,9 @@
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -1023,7 +996,9 @@
       <c r="B2" s="1">
         <v>12841</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>8844</v>
+      </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1035,7 +1010,9 @@
       <c r="B3" s="1">
         <v>12843</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>8917</v>
+      </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -1047,7 +1024,9 @@
       <c r="B4" s="1">
         <v>12816</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>8703</v>
+      </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1059,7 +1038,9 @@
       <c r="B5" s="1">
         <v>13028</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>9020</v>
+      </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1071,7 +1052,9 @@
       <c r="B6" s="1">
         <v>12880</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>9197</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -1083,7 +1066,9 @@
       <c r="B7" s="1">
         <v>13044</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>8943</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1095,7 +1080,9 @@
       <c r="B8" s="1">
         <v>12862</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>9048</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -1107,7 +1094,9 @@
       <c r="B9" s="1">
         <v>13071</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>9011</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1119,7 +1108,9 @@
       <c r="B10" s="1">
         <v>12739</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>9055</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -1131,7 +1122,9 @@
       <c r="B11" s="1">
         <v>12909</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>8898</v>
+      </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1144,9 +1137,9 @@
         <f>AVERAGE(B2:B11)</f>
         <v>12903.3</v>
       </c>
-      <c r="C12" s="3" t="e">
+      <c r="C12" s="3">
         <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>8963.6</v>
       </c>
       <c r="D12" s="3" t="e">
         <f t="shared" ref="D12" si="1">AVERAGE(D2:D11)</f>
@@ -1173,9 +1166,9 @@
         <f>_xlfn.VAR.S(B2:B11)</f>
         <v>11987.12222222222</v>
       </c>
-      <c r="C13" s="3" t="e">
+      <c r="C13" s="3">
         <f t="shared" ref="C13:G13" si="2">_xlfn.VAR.S(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>18277.377777777776</v>
       </c>
       <c r="D13" s="3" t="e">
         <f t="shared" ref="D13" si="3">_xlfn.VAR.S(D2:D11)</f>
@@ -1201,9 +1194,9 @@
       <c r="B14" s="1">
         <v>0</v>
       </c>
-      <c r="C14" s="1" t="e">
+      <c r="C14" s="1">
         <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>1</v>
       </c>
       <c r="D14" s="1" t="e">
         <f t="shared" ref="D14:G14" si="4">1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
@@ -1229,9 +1222,9 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="e">
+      <c r="C15" s="1">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>1.4395220670266409</v>
       </c>
       <c r="D15" s="1" t="e">
         <f>C12/D12</f>
@@ -1257,9 +1250,9 @@
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="e">
+      <c r="C16" s="1">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>1.4395220670266409</v>
       </c>
       <c r="D16" s="1" t="e">
         <f>B12/D12</f>
@@ -1298,8 +1291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1311,7 +1304,9 @@
       <c r="B1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -1324,7 +1319,9 @@
       <c r="B2" s="1">
         <v>7010</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="1">
+        <v>5553</v>
+      </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -1337,7 +1334,9 @@
       <c r="B3" s="1">
         <v>7079</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="1">
+        <v>5561</v>
+      </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -1350,7 +1349,9 @@
       <c r="B4" s="1">
         <v>6982</v>
       </c>
-      <c r="C4" s="1"/>
+      <c r="C4" s="1">
+        <v>5600</v>
+      </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -1363,7 +1364,9 @@
       <c r="B5" s="1">
         <v>7130</v>
       </c>
-      <c r="C5" s="1"/>
+      <c r="C5" s="1">
+        <v>5607</v>
+      </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -1376,7 +1379,9 @@
       <c r="B6" s="1">
         <v>7128</v>
       </c>
-      <c r="C6" s="1"/>
+      <c r="C6" s="1">
+        <v>5577</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -1389,7 +1394,9 @@
       <c r="B7" s="1">
         <v>7113</v>
       </c>
-      <c r="C7" s="1"/>
+      <c r="C7" s="1">
+        <v>5598</v>
+      </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -1402,7 +1409,9 @@
       <c r="B8" s="1">
         <v>7150</v>
       </c>
-      <c r="C8" s="1"/>
+      <c r="C8" s="1">
+        <v>5617</v>
+      </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1415,7 +1424,9 @@
       <c r="B9" s="1">
         <v>7155</v>
       </c>
-      <c r="C9" s="1"/>
+      <c r="C9" s="1">
+        <v>5560</v>
+      </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
@@ -1428,7 +1439,9 @@
       <c r="B10" s="1">
         <v>7138</v>
       </c>
-      <c r="C10" s="1"/>
+      <c r="C10" s="1">
+        <v>5563</v>
+      </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -1441,7 +1454,9 @@
       <c r="B11" s="1">
         <v>7006</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>5573</v>
+      </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -1455,9 +1470,9 @@
         <f>AVERAGE(B2:B11)</f>
         <v>7089.1</v>
       </c>
-      <c r="C12" s="3" t="e">
+      <c r="C12" s="3">
         <f t="shared" ref="C12:G12" si="0">AVERAGE(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>5580.9</v>
       </c>
       <c r="D12" s="3" t="e">
         <f t="shared" si="0"/>
@@ -1484,9 +1499,9 @@
         <f>_xlfn.VAR.S(B2:B11)</f>
         <v>4326.0999999999995</v>
       </c>
-      <c r="C13" s="3" t="e">
+      <c r="C13" s="3">
         <f t="shared" ref="C13:G13" si="1">_xlfn.VAR.S(C2:C11)</f>
-        <v>#DIV/0!</v>
+        <v>516.76666666666677</v>
       </c>
       <c r="D13" s="3" t="e">
         <f t="shared" si="1"/>
@@ -1512,9 +1527,9 @@
       <c r="B14" s="1">
         <v>0</v>
       </c>
-      <c r="C14" s="1" t="e">
+      <c r="C14" s="1">
         <f>1-_xlfn.T.TEST(B2:B11,C2:C11,2,3)</f>
-        <v>#DIV/0!</v>
+        <v>0.99999999999999944</v>
       </c>
       <c r="D14" s="1" t="e">
         <f>1-_xlfn.T.TEST(C2:C11,D2:D11,2,3)</f>
@@ -1540,9 +1555,9 @@
       <c r="B15" s="1">
         <v>1</v>
       </c>
-      <c r="C15" s="1" t="e">
+      <c r="C15" s="1">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>1.2702431507462955</v>
       </c>
       <c r="D15" s="1" t="e">
         <f>C12/D12</f>
@@ -1568,9 +1583,9 @@
       <c r="B16" s="1">
         <v>1</v>
       </c>
-      <c r="C16" s="1" t="e">
+      <c r="C16" s="1">
         <f>B12/C12</f>
-        <v>#DIV/0!</v>
+        <v>1.2702431507462955</v>
       </c>
       <c r="D16" s="1" t="e">
         <f>B12/D12</f>

</xml_diff>